<commit_message>
Major Changes in the POM and Excel reader
</commit_message>
<xml_diff>
--- a/XAP_TOP_10/src/main/java/com/legacy/testDataFile/TestData.xlsx
+++ b/XAP_TOP_10/src/main/java/com/legacy/testDataFile/TestData.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20010" windowHeight="7860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2460" windowWidth="14790" windowHeight="6345"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K19"/>
 </workbook>
 </file>
 
@@ -151,8 +152,36 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -450,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>